<commit_message>
fix start and end date in daily schedule
</commit_message>
<xml_diff>
--- a/data/test_data_daily_schedule.xlsx
+++ b/data/test_data_daily_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rizfan\Documents\project\vmi\surgery\backend_surgery_fastapi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E237A15-B7D7-4985-A5D8-B3280A50F53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD3342-26F9-4C07-8225-BFFC5AF9FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1398,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244F6AE9-728D-E247-A126-31EDB904D4D8}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3">
-        <v>44918</v>
+        <v>45607</v>
       </c>
       <c r="B2" t="s">
         <v>241</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3">
-        <v>44922</v>
+        <v>45608</v>
       </c>
       <c r="B3" t="s">
         <v>242</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3">
-        <v>44922</v>
+        <v>45609</v>
       </c>
       <c r="B4" t="s">
         <v>243</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="3">
-        <v>44923</v>
+        <v>45610</v>
       </c>
       <c r="B5" t="s">
         <v>244</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="3">
-        <v>44923</v>
+        <v>45611</v>
       </c>
       <c r="B6" t="s">
         <v>245</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="3">
-        <v>44923</v>
+        <v>45614</v>
       </c>
       <c r="B7" t="s">
         <v>246</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3">
-        <v>44923</v>
+        <v>45615</v>
       </c>
       <c r="B8" t="s">
         <v>247</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3">
-        <v>44924</v>
+        <v>45616</v>
       </c>
       <c r="B9" t="s">
         <v>248</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3">
-        <v>44924</v>
+        <v>45617</v>
       </c>
       <c r="B10" t="s">
         <v>249</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="3">
-        <v>44924</v>
+        <v>45618</v>
       </c>
       <c r="B11" t="s">
         <v>250</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="3">
-        <v>44925</v>
+        <v>45621</v>
       </c>
       <c r="B12" t="s">
         <v>251</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="3">
-        <v>44925</v>
+        <v>45622</v>
       </c>
       <c r="B13" t="s">
         <v>252</v>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="3">
-        <v>44925</v>
+        <v>45623</v>
       </c>
       <c r="B14" t="s">
         <v>253</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="3">
-        <v>44926</v>
+        <v>45624</v>
       </c>
       <c r="B15" t="s">
         <v>254</v>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="3">
-        <v>44927</v>
+        <v>45625</v>
       </c>
       <c r="B16" t="s">
         <v>255</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="3">
-        <v>44929</v>
+        <v>45628</v>
       </c>
       <c r="B17" t="s">
         <v>255</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="3">
-        <v>44929</v>
+        <v>45629</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="3">
-        <v>44929</v>
+        <v>45630</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="3">
-        <v>44929</v>
+        <v>45631</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="3">
-        <v>44929</v>
+        <v>45632</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="3">
-        <v>44929</v>
+        <v>45635</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -2388,7 +2388,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="3">
-        <v>44929</v>
+        <v>45636</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="3">
-        <v>44929</v>
+        <v>45637</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="3">
-        <v>44929</v>
+        <v>45638</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="3">
-        <v>44929</v>
+        <v>45639</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="3">
-        <v>44837</v>
+        <v>45642</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="3">
-        <v>44866</v>
+        <v>45643</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="3">
-        <v>44866</v>
+        <v>45644</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="3">
-        <v>44880</v>
+        <v>45645</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -2740,7 +2740,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="3">
-        <v>44893</v>
+        <v>45646</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="3">
-        <v>44895</v>
+        <v>45649</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="3">
-        <v>44896</v>
+        <v>45650</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="3">
-        <v>44908</v>
+        <v>45651</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -2916,7 +2916,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="3">
-        <v>44910</v>
+        <v>45652</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="3">
-        <v>44917</v>
+        <v>45653</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="3">
-        <v>44929</v>
+        <v>45656</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="3">
-        <v>44929</v>
+        <v>45657</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -3089,7 +3089,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="3">
-        <v>44929</v>
+        <v>45658</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="3">
-        <v>44929</v>
+        <v>45659</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="3">
-        <v>44929</v>
+        <v>45660</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="3">
-        <v>44837</v>
+        <v>45663</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="3">
-        <v>44866</v>
+        <v>45664</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" s="3">
-        <v>44866</v>
+        <v>45665</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="3">
-        <v>44880</v>
+        <v>45666</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="3">
-        <v>44893</v>
+        <v>45667</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="3">
-        <v>44895</v>
+        <v>45670</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="3">
-        <v>44896</v>
+        <v>45674</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -3523,7 +3523,7 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" s="3">
-        <v>44908</v>
+        <v>45678</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="3">
-        <v>44910</v>
+        <v>45682</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="3">
-        <v>44917</v>
+        <v>45686</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
improve master plan -> AI OT Manager Testing III (20241113)
</commit_message>
<xml_diff>
--- a/data/test_data_daily_schedule.xlsx
+++ b/data/test_data_daily_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rizfan\Documents\project\vmi\surgery\backend_surgery_fastapi\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angga\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD3342-26F9-4C07-8225-BFFC5AF9FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068E1162-F931-4450-A2EE-D6F81D39CF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,6 +37,9 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="288">
+  <si>
+    <t>BOOKING_DATE</t>
+  </si>
   <si>
     <t>MRN</t>
   </si>
@@ -1001,9 +1006,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>BOOKING DATE</t>
   </si>
 </sst>
 </file>
@@ -1398,2259 +1400,2259 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244F6AE9-728D-E247-A126-31EDB904D4D8}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="E35" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="28.25" customWidth="1"/>
-    <col min="5" max="5" width="60.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="73.25" customWidth="1"/>
+    <col min="1" max="1" width="28.296875" customWidth="1"/>
+    <col min="5" max="5" width="60.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="73.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>287</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3">
-        <v>45607</v>
+        <v>44918</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C2" s="4">
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3">
-        <v>45608</v>
+        <v>44922</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C3" s="4">
         <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3">
-        <v>45609</v>
+        <v>44922</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C4" s="4">
         <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="N4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="3">
-        <v>45610</v>
+        <v>44923</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C5" s="4">
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="M5" t="s">
+        <v>139</v>
+      </c>
+      <c r="N5" t="s">
         <v>138</v>
-      </c>
-      <c r="N5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="3">
-        <v>45611</v>
+        <v>44923</v>
       </c>
       <c r="B6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C6" s="4">
         <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M6" t="s">
+        <v>139</v>
+      </c>
+      <c r="N6" t="s">
         <v>138</v>
-      </c>
-      <c r="N6" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="3">
-        <v>45614</v>
+        <v>44923</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C7" s="4">
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M7" t="s">
+        <v>139</v>
+      </c>
+      <c r="N7" t="s">
         <v>138</v>
-      </c>
-      <c r="N7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3">
-        <v>45615</v>
+        <v>44923</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C8" s="4">
         <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3">
-        <v>45616</v>
+        <v>44924</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C9" s="4">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3">
-        <v>45617</v>
+        <v>44924</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C10" s="4">
         <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="3">
-        <v>45618</v>
+        <v>44924</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C11" s="4">
         <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="3">
-        <v>45621</v>
+        <v>44925</v>
       </c>
       <c r="B12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C12" s="4">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="3">
-        <v>45622</v>
+        <v>44925</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C13" s="4">
         <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="M13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="3">
-        <v>45623</v>
+        <v>44925</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C14" s="4">
         <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L14" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="3">
-        <v>45624</v>
+        <v>44926</v>
       </c>
       <c r="B15" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C15" s="4">
         <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F15" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="3">
-        <v>45625</v>
+        <v>44927</v>
       </c>
       <c r="B16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C16" s="4">
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F16" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="3">
-        <v>45628</v>
+        <v>44929</v>
       </c>
       <c r="B17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C17" s="4">
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K17" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="3">
-        <v>45629</v>
+        <v>44929</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="4">
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K18" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="3">
-        <v>45630</v>
+        <v>44929</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" s="4">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="3">
-        <v>45631</v>
+        <v>44929</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" s="4">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="3">
-        <v>45632</v>
+        <v>44929</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4">
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K21" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="M21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O21" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="3">
-        <v>45635</v>
+        <v>44929</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="4">
         <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="3">
-        <v>45636</v>
+        <v>44929</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" s="4">
         <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="3">
-        <v>45637</v>
+        <v>44929</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4">
         <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K24" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L24" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="3">
-        <v>45638</v>
+        <v>44929</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C25" s="4">
         <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K25" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L25" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="N25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="3">
-        <v>45639</v>
+        <v>44929</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="4">
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K26" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M26" t="s">
+        <v>164</v>
+      </c>
+      <c r="N26" t="s">
         <v>163</v>
-      </c>
-      <c r="N26" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="3">
-        <v>45642</v>
+        <v>44837</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C27" s="4">
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G27" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J27" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K27" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L27" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M27" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="3">
-        <v>45643</v>
+        <v>44866</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4">
         <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K28" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M28" t="s">
+        <v>137</v>
+      </c>
+      <c r="N28" t="s">
         <v>136</v>
-      </c>
-      <c r="N28" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="3">
-        <v>45644</v>
+        <v>44866</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C29" s="4">
         <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K29" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M29" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="3">
-        <v>45645</v>
+        <v>44880</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C30" s="4">
         <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G30" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L30" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="3">
-        <v>45646</v>
+        <v>44893</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" s="4">
         <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J31" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="3">
-        <v>45649</v>
+        <v>44895</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C32" s="4">
         <v>73</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K32" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L32" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M32" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="3">
-        <v>45650</v>
+        <v>44896</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C33" s="4">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I33" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J33" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K33" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L33" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M33" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="N33" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="3">
-        <v>45651</v>
+        <v>44908</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" s="4">
         <v>80</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I34" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K34" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L34" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="3">
-        <v>45652</v>
+        <v>44910</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" s="4">
         <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F35" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K35" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L35" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="3">
-        <v>45653</v>
+        <v>44917</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C36" s="4">
         <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F36" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I36" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J36" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K36" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L36" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N36" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="3">
-        <v>45656</v>
+        <v>44929</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" s="4">
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G37" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J37" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K37" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L37" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M37" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N37" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="3">
-        <v>45657</v>
+        <v>44929</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C38" s="4">
         <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G38" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J38" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K38" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L38" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N38" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="3">
-        <v>45658</v>
+        <v>44929</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C39" s="4">
         <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F39" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G39" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I39" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J39" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K39" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M39" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N39" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="3">
-        <v>45659</v>
+        <v>44929</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40" s="4">
         <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I40" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L40" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N40" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="3">
-        <v>45660</v>
+        <v>44929</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C41" s="4">
         <v>57</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G41" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I41" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J41" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K41" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L41" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="M41" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N41" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="3">
-        <v>45663</v>
+        <v>44837</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C42" s="4">
         <v>79</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G42" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I42" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J42" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K42" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L42" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M42" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N42" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="3">
-        <v>45664</v>
+        <v>44866</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C43" s="4">
         <v>27</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F43" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G43" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H43" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I43" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J43" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K43" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L43" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N43" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:14">
       <c r="A44" s="3">
-        <v>45665</v>
+        <v>44866</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C44" s="4">
         <v>39</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F44" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G44" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I44" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J44" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K44" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L44" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M44" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N44" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="3">
-        <v>45666</v>
+        <v>44880</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C45" s="4">
         <v>72</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F45" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G45" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H45" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I45" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J45" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K45" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L45" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M45" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N45" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="3">
-        <v>45667</v>
+        <v>44893</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C46" s="4">
         <v>60</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F46" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K46" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L46" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M46" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="3">
-        <v>45670</v>
+        <v>44895</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C47" s="4">
         <v>80</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G47" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H47" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J47" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K47" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L47" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M47" t="s">
+        <v>190</v>
+      </c>
+      <c r="N47" t="s">
         <v>189</v>
-      </c>
-      <c r="N47" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="3">
-        <v>45674</v>
+        <v>44896</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C48" s="4">
         <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F48" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G48" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" t="s">
         <v>17</v>
       </c>
-      <c r="H48" t="s">
-        <v>16</v>
-      </c>
       <c r="I48" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J48" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K48" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M48" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N48" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" s="3">
-        <v>45678</v>
+        <v>44908</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C49" s="4">
         <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F49" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H49" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I49" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K49" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L49" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N49" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="3">
-        <v>45682</v>
+        <v>44910</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C50" s="4">
         <v>56</v>
       </c>
       <c r="D50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F50" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" t="s">
         <v>17</v>
       </c>
-      <c r="H50" t="s">
-        <v>16</v>
-      </c>
       <c r="I50" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J50" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K50" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M50" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N50" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="3">
-        <v>45686</v>
+        <v>44917</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C51" s="4">
         <v>75</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F51" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G51" t="s">
+        <v>18</v>
+      </c>
+      <c r="H51" t="s">
         <v>17</v>
       </c>
-      <c r="H51" t="s">
-        <v>16</v>
-      </c>
       <c r="I51" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J51" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K51" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L51" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M51" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N51" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix generate schedule & view schedule - AI OT Manager Testing IV (20241127)
</commit_message>
<xml_diff>
--- a/data/test_data_daily_schedule.xlsx
+++ b/data/test_data_daily_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angga\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\vmi\surgery\backend_surgery_fastapi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068E1162-F931-4450-A2EE-D6F81D39CF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29900892-73ED-4ED9-8D3B-4B0F71085B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="288">
   <si>
-    <t>BOOKING_DATE</t>
-  </si>
-  <si>
     <t>MRN</t>
   </si>
   <si>
@@ -1006,6 +1003,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>BOOKING DATE</t>
   </si>
 </sst>
 </file>
@@ -1400,62 +1400,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244F6AE9-728D-E247-A126-31EDB904D4D8}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E35" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H51"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.296875" customWidth="1"/>
-    <col min="5" max="5" width="60.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="73.296875" customWidth="1"/>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
+    <col min="5" max="5" width="60.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="73.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1463,43 +1461,43 @@
         <v>44918</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" s="4">
         <v>34</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
       <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
         <v>116</v>
       </c>
-      <c r="I2" t="s">
-        <v>117</v>
-      </c>
       <c r="J2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" t="s">
         <v>133</v>
-      </c>
-      <c r="N2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1507,43 +1505,43 @@
         <v>44922</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C3" s="4">
         <v>52</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
       <c r="H3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" t="s">
         <v>135</v>
-      </c>
-      <c r="N3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1551,46 +1549,46 @@
         <v>44922</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="4">
         <v>68</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>266</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" t="s">
-        <v>267</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
       <c r="K4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N4" t="s">
         <v>137</v>
       </c>
-      <c r="N4" t="s">
-        <v>138</v>
-      </c>
       <c r="O4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1598,43 +1596,43 @@
         <v>44923</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C5" s="4">
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
       <c r="K5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1642,43 +1640,43 @@
         <v>44923</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" s="4">
         <v>68</v>
       </c>
       <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" t="s">
-        <v>269</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
       <c r="K6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1686,43 +1684,43 @@
         <v>44923</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C7" s="4">
         <v>60</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>269</v>
+      </c>
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
-        <v>270</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
       <c r="K7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1730,43 +1728,43 @@
         <v>44923</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C8" s="4">
         <v>67</v>
       </c>
       <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8" t="s">
+        <v>270</v>
+      </c>
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
-        <v>258</v>
-      </c>
-      <c r="F8" t="s">
-        <v>271</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
       <c r="I8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N8" t="s">
         <v>140</v>
-      </c>
-      <c r="N8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1774,43 +1772,43 @@
         <v>44924</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C9" s="4">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M9" t="s">
+        <v>141</v>
+      </c>
+      <c r="N9" t="s">
         <v>142</v>
-      </c>
-      <c r="N9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1818,43 +1816,43 @@
         <v>44924</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C10" s="4">
         <v>67</v>
       </c>
       <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" t="s">
+        <v>272</v>
+      </c>
+      <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
-        <v>260</v>
-      </c>
-      <c r="F10" t="s">
-        <v>273</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J10" t="s">
-        <v>18</v>
-      </c>
       <c r="K10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1862,43 +1860,43 @@
         <v>44924</v>
       </c>
       <c r="B11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C11" s="4">
         <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
         <v>16</v>
       </c>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
       <c r="I11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M11" t="s">
+        <v>144</v>
+      </c>
+      <c r="N11" t="s">
         <v>145</v>
-      </c>
-      <c r="N11" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1906,43 +1904,43 @@
         <v>44925</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C12" s="4">
         <v>13</v>
       </c>
       <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>261</v>
+      </c>
+      <c r="F12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
-        <v>262</v>
-      </c>
-      <c r="F12" t="s">
-        <v>275</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>16</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" t="s">
         <v>17</v>
       </c>
-      <c r="I12" t="s">
-        <v>122</v>
-      </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
       <c r="K12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1950,43 +1948,43 @@
         <v>44925</v>
       </c>
       <c r="B13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C13" s="4">
         <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" t="s">
         <v>17</v>
       </c>
-      <c r="I13" t="s">
-        <v>122</v>
-      </c>
-      <c r="J13" t="s">
-        <v>18</v>
-      </c>
       <c r="K13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1994,43 +1992,43 @@
         <v>44925</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C14" s="4">
         <v>63</v>
       </c>
       <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>276</v>
+      </c>
+      <c r="G14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" t="s">
-        <v>277</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>16</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" t="s">
         <v>17</v>
       </c>
-      <c r="I14" t="s">
-        <v>122</v>
-      </c>
-      <c r="J14" t="s">
-        <v>18</v>
-      </c>
       <c r="K14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2038,43 +2036,43 @@
         <v>44926</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C15" s="4">
         <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
         <v>16</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15" t="s">
         <v>17</v>
       </c>
-      <c r="I15" t="s">
-        <v>122</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
       <c r="K15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -2082,43 +2080,43 @@
         <v>44927</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C16" s="4">
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M16" t="s">
+        <v>149</v>
+      </c>
+      <c r="N16" t="s">
         <v>150</v>
-      </c>
-      <c r="N16" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -2126,43 +2124,43 @@
         <v>44929</v>
       </c>
       <c r="B17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C17" s="4">
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" t="s">
         <v>115</v>
       </c>
-      <c r="H17" t="s">
-        <v>116</v>
-      </c>
       <c r="I17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M17" t="s">
+        <v>149</v>
+      </c>
+      <c r="N17" t="s">
         <v>150</v>
-      </c>
-      <c r="N17" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -2170,43 +2168,43 @@
         <v>44929</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4">
         <v>32</v>
       </c>
       <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
         <v>16</v>
       </c>
-      <c r="H18" t="s">
-        <v>17</v>
-      </c>
       <c r="I18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -2214,43 +2212,43 @@
         <v>44929</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="4">
         <v>2</v>
       </c>
       <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>16</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J19" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J19" t="s">
-        <v>18</v>
-      </c>
       <c r="K19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M19" t="s">
+        <v>152</v>
+      </c>
+      <c r="N19" t="s">
         <v>153</v>
-      </c>
-      <c r="N19" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -2258,43 +2256,43 @@
         <v>44929</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="4">
         <v>34</v>
       </c>
       <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
         <v>15</v>
       </c>
-      <c r="E20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>16</v>
       </c>
-      <c r="H20" t="s">
-        <v>17</v>
-      </c>
       <c r="I20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N20" t="s">
         <v>155</v>
-      </c>
-      <c r="N20" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -2302,46 +2300,46 @@
         <v>44929</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="4">
         <v>68</v>
       </c>
       <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" t="s">
         <v>15</v>
       </c>
-      <c r="E21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>16</v>
       </c>
-      <c r="H21" t="s">
-        <v>17</v>
-      </c>
       <c r="I21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2349,43 +2347,43 @@
         <v>44929</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="4">
         <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
         <v>16</v>
       </c>
-      <c r="H22" t="s">
-        <v>17</v>
-      </c>
       <c r="I22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2393,43 +2391,43 @@
         <v>44929</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="4">
         <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M23" t="s">
+        <v>157</v>
+      </c>
+      <c r="N23" t="s">
         <v>158</v>
-      </c>
-      <c r="N23" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2437,43 +2435,43 @@
         <v>44929</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="4">
         <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M24" t="s">
+        <v>159</v>
+      </c>
+      <c r="N24" t="s">
         <v>160</v>
-      </c>
-      <c r="N24" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -2481,43 +2479,43 @@
         <v>44929</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4">
         <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" t="s">
         <v>115</v>
       </c>
-      <c r="H25" t="s">
-        <v>116</v>
-      </c>
       <c r="I25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M25" t="s">
+        <v>161</v>
+      </c>
+      <c r="N25" t="s">
         <v>162</v>
-      </c>
-      <c r="N25" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -2525,43 +2523,43 @@
         <v>44929</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4">
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -2569,43 +2567,43 @@
         <v>44837</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="4">
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" t="s">
         <v>115</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>116</v>
       </c>
-      <c r="I27" t="s">
-        <v>117</v>
-      </c>
       <c r="J27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M27" t="s">
+        <v>164</v>
+      </c>
+      <c r="N27" t="s">
         <v>165</v>
-      </c>
-      <c r="N27" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -2613,43 +2611,43 @@
         <v>44866</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="4">
         <v>67</v>
       </c>
       <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" t="s">
         <v>15</v>
       </c>
-      <c r="E28" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>16</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
+        <v>121</v>
+      </c>
+      <c r="J28" t="s">
         <v>17</v>
       </c>
-      <c r="I28" t="s">
-        <v>122</v>
-      </c>
-      <c r="J28" t="s">
-        <v>18</v>
-      </c>
       <c r="K28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2657,43 +2655,43 @@
         <v>44866</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4">
         <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2701,43 +2699,43 @@
         <v>44880</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="4">
         <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" t="s">
         <v>115</v>
       </c>
-      <c r="H30" t="s">
-        <v>116</v>
-      </c>
       <c r="I30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M30" t="s">
+        <v>167</v>
+      </c>
+      <c r="N30" t="s">
         <v>168</v>
-      </c>
-      <c r="N30" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -2745,43 +2743,43 @@
         <v>44893</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="4">
         <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" t="s">
         <v>115</v>
       </c>
-      <c r="H31" t="s">
-        <v>116</v>
-      </c>
       <c r="I31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2789,43 +2787,43 @@
         <v>44895</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="4">
         <v>73</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
         <v>16</v>
       </c>
-      <c r="H32" t="s">
-        <v>17</v>
-      </c>
       <c r="I32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M32" t="s">
+        <v>159</v>
+      </c>
+      <c r="N32" t="s">
         <v>160</v>
-      </c>
-      <c r="N32" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2833,43 +2831,43 @@
         <v>44896</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="4">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" t="s">
         <v>115</v>
       </c>
-      <c r="H33" t="s">
-        <v>116</v>
-      </c>
       <c r="I33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M33" t="s">
+        <v>170</v>
+      </c>
+      <c r="N33" t="s">
         <v>171</v>
-      </c>
-      <c r="N33" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2877,43 +2875,43 @@
         <v>44908</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="4">
         <v>80</v>
       </c>
       <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" t="s">
         <v>15</v>
       </c>
-      <c r="E34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>16</v>
       </c>
-      <c r="H34" t="s">
-        <v>17</v>
-      </c>
       <c r="I34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M34" t="s">
+        <v>172</v>
+      </c>
+      <c r="N34" t="s">
         <v>173</v>
-      </c>
-      <c r="N34" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2921,43 +2919,43 @@
         <v>44910</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="4">
         <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M35" t="s">
+        <v>174</v>
+      </c>
+      <c r="N35" t="s">
         <v>175</v>
-      </c>
-      <c r="N35" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2965,43 +2963,43 @@
         <v>44917</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="4">
         <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -3009,43 +3007,43 @@
         <v>44929</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="4">
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K37" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M37" t="s">
+        <v>177</v>
+      </c>
+      <c r="N37" t="s">
         <v>178</v>
-      </c>
-      <c r="N37" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -3053,40 +3051,40 @@
         <v>44929</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="4">
         <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M38" t="s">
+        <v>159</v>
+      </c>
+      <c r="N38" t="s">
         <v>160</v>
-      </c>
-      <c r="N38" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -3094,43 +3092,43 @@
         <v>44929</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" s="4">
         <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M39" t="s">
+        <v>179</v>
+      </c>
+      <c r="N39" t="s">
         <v>180</v>
-      </c>
-      <c r="N39" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -3138,40 +3136,40 @@
         <v>44929</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="4">
         <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M40" t="s">
+        <v>159</v>
+      </c>
+      <c r="N40" t="s">
         <v>160</v>
-      </c>
-      <c r="N40" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -3179,43 +3177,43 @@
         <v>44929</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="4">
         <v>57</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M41" t="s">
+        <v>181</v>
+      </c>
+      <c r="N41" t="s">
         <v>182</v>
-      </c>
-      <c r="N41" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -3223,43 +3221,43 @@
         <v>44837</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" s="4">
         <v>79</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -3267,43 +3265,43 @@
         <v>44866</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="4">
         <v>27</v>
       </c>
       <c r="D43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M43" t="s">
+        <v>184</v>
+      </c>
+      <c r="N43" t="s">
         <v>185</v>
-      </c>
-      <c r="N43" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -3311,43 +3309,43 @@
         <v>44866</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="4">
         <v>39</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M44" t="s">
+        <v>184</v>
+      </c>
+      <c r="N44" t="s">
         <v>185</v>
-      </c>
-      <c r="N44" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -3355,43 +3353,43 @@
         <v>44880</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="4">
         <v>72</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -3399,40 +3397,40 @@
         <v>44893</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="4">
         <v>60</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M46" t="s">
+        <v>187</v>
+      </c>
+      <c r="N46" t="s">
         <v>188</v>
-      </c>
-      <c r="N46" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -3440,43 +3438,43 @@
         <v>44895</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="4">
         <v>80</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -3484,43 +3482,43 @@
         <v>44896</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="4">
         <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H48" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J48" t="s">
         <v>17</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J48" t="s">
-        <v>18</v>
-      </c>
       <c r="K48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M48" t="s">
+        <v>190</v>
+      </c>
+      <c r="N48" t="s">
         <v>191</v>
-      </c>
-      <c r="N48" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -3528,43 +3526,43 @@
         <v>44908</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="4">
         <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M49" t="s">
+        <v>192</v>
+      </c>
+      <c r="N49" t="s">
         <v>193</v>
-      </c>
-      <c r="N49" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -3572,43 +3570,43 @@
         <v>44910</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="4">
         <v>56</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" t="s">
+        <v>121</v>
+      </c>
+      <c r="J50" t="s">
         <v>17</v>
       </c>
-      <c r="I50" t="s">
-        <v>122</v>
-      </c>
-      <c r="J50" t="s">
-        <v>18</v>
-      </c>
       <c r="K50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -3616,43 +3614,43 @@
         <v>44917</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" s="4">
         <v>75</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J51" t="s">
         <v>17</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J51" t="s">
-        <v>18</v>
-      </c>
       <c r="K51" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>